<commit_message>
try Test Cases with some correction
</commit_message>
<xml_diff>
--- a/try.tests/try Test Cases.xlsx
+++ b/try.tests/try Test Cases.xlsx
@@ -185,9 +185,6 @@
     <t>1.Type URL http://automationpractice.com/</t>
   </si>
   <si>
-    <t>9.Verify is total price has been charged corectly</t>
-  </si>
-  <si>
     <t xml:space="preserve">1.Page is successfully opened </t>
   </si>
   <si>
@@ -212,9 +209,6 @@
     <t>3.Item page is loaded</t>
   </si>
   <si>
-    <t>4.Items with choosen properties are in the cart</t>
-  </si>
-  <si>
     <t>5.Pop-up window is closed</t>
   </si>
   <si>
@@ -225,9 +219,6 @@
   </si>
   <si>
     <t>8.Checkout page is loaded</t>
-  </si>
-  <si>
-    <t>9.Total price is charged corectly</t>
   </si>
   <si>
     <t>1. Page is opened
@@ -235,6 +226,15 @@
   </si>
   <si>
     <t>2.Hover over  "Dresses" an choose 'Casual dresses'</t>
+  </si>
+  <si>
+    <t>4.Items with chosen properties are in the cart</t>
+  </si>
+  <si>
+    <t>9.Verify is total price has been charged correctly</t>
+  </si>
+  <si>
+    <t>9.Total price is charged correctly</t>
   </si>
 </sst>
 </file>
@@ -1080,7 +1080,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B3:M31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I17" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="H24" workbookViewId="0">
       <selection activeCell="J26" sqref="J26"/>
     </sheetView>
   </sheetViews>
@@ -1294,7 +1294,7 @@
         <v>25</v>
       </c>
       <c r="J15" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="K15" s="7" t="s">
         <v>51</v>
@@ -1376,7 +1376,7 @@
         <v>53</v>
       </c>
       <c r="K23" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="L23" s="2" t="s">
         <v>22</v>
@@ -1395,10 +1395,10 @@
       <c r="H24" s="9"/>
       <c r="I24" s="9"/>
       <c r="J24" s="7" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="K24" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="L24" s="7" t="s">
         <v>22</v>
@@ -1415,10 +1415,10 @@
       <c r="H25" s="9"/>
       <c r="I25" s="9"/>
       <c r="J25" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="K25" s="7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="L25" s="7" t="s">
         <v>22</v>
@@ -1435,10 +1435,10 @@
       <c r="H26" s="9"/>
       <c r="I26" s="9"/>
       <c r="J26" s="7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="K26" s="7" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="L26" s="7" t="s">
         <v>22</v>
@@ -1455,10 +1455,10 @@
       <c r="H27" s="9"/>
       <c r="I27" s="9"/>
       <c r="J27" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="K27" s="7" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="L27" s="7" t="s">
         <v>22</v>
@@ -1475,10 +1475,10 @@
       <c r="H28" s="9"/>
       <c r="I28" s="9"/>
       <c r="J28" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="K28" s="7" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="L28" s="7" t="s">
         <v>22</v>
@@ -1495,10 +1495,10 @@
       <c r="H29" s="9"/>
       <c r="I29" s="9"/>
       <c r="J29" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="K29" s="7" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="L29" s="7" t="s">
         <v>22</v>
@@ -1518,7 +1518,7 @@
         <v>52</v>
       </c>
       <c r="K30" s="7" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="L30" s="7" t="s">
         <v>22</v>
@@ -1535,10 +1535,10 @@
       <c r="H31" s="3"/>
       <c r="I31" s="3"/>
       <c r="J31" s="4" t="s">
-        <v>54</v>
+        <v>69</v>
       </c>
       <c r="K31" s="4" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="L31" s="4" t="s">
         <v>22</v>

</xml_diff>

<commit_message>
Zmodyfikowany na próbę plik xlsx
</commit_message>
<xml_diff>
--- a/try.tests/try Test Cases.xlsx
+++ b/try.tests/try Test Cases.xlsx
@@ -118,9 +118,6 @@
     <t>According to the specification, page should display same results as for 't-shirt' search</t>
   </si>
   <si>
-    <t>Bug report</t>
-  </si>
-  <si>
     <t>Title</t>
   </si>
   <si>
@@ -235,6 +232,9 @@
   </si>
   <si>
     <t>9.Total price is charged correctly</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bug report </t>
   </si>
 </sst>
 </file>
@@ -1080,8 +1080,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B3:M31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H24" workbookViewId="0">
-      <selection activeCell="J26" sqref="J26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1227,7 +1227,7 @@
     </row>
     <row r="11" spans="2:13" ht="15">
       <c r="B11" s="1" t="s">
-        <v>32</v>
+        <v>70</v>
       </c>
     </row>
     <row r="14" spans="2:13" ht="15.75">
@@ -1235,10 +1235,10 @@
         <v>0</v>
       </c>
       <c r="C14" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D14" s="6" t="s">
         <v>33</v>
-      </c>
-      <c r="D14" s="6" t="s">
-        <v>34</v>
       </c>
       <c r="E14" s="6" t="s">
         <v>14</v>
@@ -1247,25 +1247,25 @@
         <v>15</v>
       </c>
       <c r="G14" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H14" s="6" t="s">
         <v>18</v>
       </c>
       <c r="I14" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="J14" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="J14" s="6" t="s">
+      <c r="K14" s="6" t="s">
         <v>37</v>
-      </c>
-      <c r="K14" s="6" t="s">
-        <v>38</v>
       </c>
       <c r="L14" s="6" t="s">
         <v>4</v>
       </c>
       <c r="M14" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="15" spans="2:13" ht="139.5" customHeight="1">
@@ -1273,19 +1273,19 @@
         <v>6</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D15" s="7" t="s">
         <v>16</v>
       </c>
       <c r="E15" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="F15" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="F15" s="7" t="s">
+      <c r="G15" s="7" t="s">
         <v>42</v>
-      </c>
-      <c r="G15" s="7" t="s">
-        <v>43</v>
       </c>
       <c r="H15" s="7" t="s">
         <v>20</v>
@@ -1294,19 +1294,19 @@
         <v>25</v>
       </c>
       <c r="J15" s="7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="K15" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="L15" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="M15" s="7"/>
     </row>
     <row r="18" spans="2:13" ht="15">
       <c r="B18" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="21" spans="2:13" ht="15.75">
@@ -1349,22 +1349,22 @@
     </row>
     <row r="23" spans="2:13" ht="45" customHeight="1">
       <c r="B23" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C23" s="2" t="s">
         <v>46</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>47</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E23" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="F23" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="F23" s="2" t="s">
+      <c r="G23" s="2" t="s">
         <v>49</v>
-      </c>
-      <c r="G23" s="2" t="s">
-        <v>50</v>
       </c>
       <c r="H23" s="2" t="s">
         <v>19</v>
@@ -1373,10 +1373,10 @@
         <v>20</v>
       </c>
       <c r="J23" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="K23" s="2" t="s">
         <v>53</v>
-      </c>
-      <c r="K23" s="2" t="s">
-        <v>54</v>
       </c>
       <c r="L23" s="2" t="s">
         <v>22</v>
@@ -1395,10 +1395,10 @@
       <c r="H24" s="9"/>
       <c r="I24" s="9"/>
       <c r="J24" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="K24" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="L24" s="7" t="s">
         <v>22</v>
@@ -1415,10 +1415,10 @@
       <c r="H25" s="9"/>
       <c r="I25" s="9"/>
       <c r="J25" s="7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="K25" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="L25" s="7" t="s">
         <v>22</v>
@@ -1435,10 +1435,10 @@
       <c r="H26" s="9"/>
       <c r="I26" s="9"/>
       <c r="J26" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="K26" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="L26" s="7" t="s">
         <v>22</v>
@@ -1455,10 +1455,10 @@
       <c r="H27" s="9"/>
       <c r="I27" s="9"/>
       <c r="J27" s="7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="K27" s="7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="L27" s="7" t="s">
         <v>22</v>
@@ -1475,10 +1475,10 @@
       <c r="H28" s="9"/>
       <c r="I28" s="9"/>
       <c r="J28" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="K28" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="L28" s="7" t="s">
         <v>22</v>
@@ -1495,10 +1495,10 @@
       <c r="H29" s="9"/>
       <c r="I29" s="9"/>
       <c r="J29" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="K29" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="L29" s="7" t="s">
         <v>22</v>
@@ -1515,10 +1515,10 @@
       <c r="H30" s="9"/>
       <c r="I30" s="9"/>
       <c r="J30" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="K30" s="7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="L30" s="7" t="s">
         <v>22</v>
@@ -1535,10 +1535,10 @@
       <c r="H31" s="3"/>
       <c r="I31" s="3"/>
       <c r="J31" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="K31" s="4" t="s">
         <v>69</v>
-      </c>
-      <c r="K31" s="4" t="s">
-        <v>70</v>
       </c>
       <c r="L31" s="4" t="s">
         <v>22</v>

</xml_diff>

<commit_message>
'try Test Cases' file correction
</commit_message>
<xml_diff>
--- a/try.tests/try Test Cases.xlsx
+++ b/try.tests/try Test Cases.xlsx
@@ -115,9 +115,6 @@
     <t>Failed</t>
   </si>
   <si>
-    <t>According to the specification, page should display same results as for 't-shirt' search</t>
-  </si>
-  <si>
     <t>Title</t>
   </si>
   <si>
@@ -235,6 +232,9 @@
   </si>
   <si>
     <t xml:space="preserve">Bug report </t>
+  </si>
+  <si>
+    <t>According to the specification, page should display the same results as for 't-shirt' search</t>
   </si>
 </sst>
 </file>
@@ -1080,8 +1080,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B3:M31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1222,12 +1222,12 @@
         <v>30</v>
       </c>
       <c r="M8" s="4" t="s">
-        <v>31</v>
+        <v>70</v>
       </c>
     </row>
     <row r="11" spans="2:13" ht="15">
       <c r="B11" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="14" spans="2:13" ht="15.75">
@@ -1235,10 +1235,10 @@
         <v>0</v>
       </c>
       <c r="C14" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D14" s="6" t="s">
         <v>32</v>
-      </c>
-      <c r="D14" s="6" t="s">
-        <v>33</v>
       </c>
       <c r="E14" s="6" t="s">
         <v>14</v>
@@ -1247,25 +1247,25 @@
         <v>15</v>
       </c>
       <c r="G14" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H14" s="6" t="s">
         <v>18</v>
       </c>
       <c r="I14" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="J14" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="J14" s="6" t="s">
+      <c r="K14" s="6" t="s">
         <v>36</v>
-      </c>
-      <c r="K14" s="6" t="s">
-        <v>37</v>
       </c>
       <c r="L14" s="6" t="s">
         <v>4</v>
       </c>
       <c r="M14" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="15" spans="2:13" ht="139.5" customHeight="1">
@@ -1273,19 +1273,19 @@
         <v>6</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D15" s="7" t="s">
         <v>16</v>
       </c>
       <c r="E15" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="F15" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="F15" s="7" t="s">
+      <c r="G15" s="7" t="s">
         <v>41</v>
-      </c>
-      <c r="G15" s="7" t="s">
-        <v>42</v>
       </c>
       <c r="H15" s="7" t="s">
         <v>20</v>
@@ -1294,19 +1294,19 @@
         <v>25</v>
       </c>
       <c r="J15" s="7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="K15" s="7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="L15" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="M15" s="7"/>
     </row>
     <row r="18" spans="2:13" ht="15">
       <c r="B18" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="21" spans="2:13" ht="15.75">
@@ -1349,22 +1349,22 @@
     </row>
     <row r="23" spans="2:13" ht="45" customHeight="1">
       <c r="B23" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C23" s="2" t="s">
         <v>45</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>46</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E23" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="F23" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="F23" s="2" t="s">
+      <c r="G23" s="2" t="s">
         <v>48</v>
-      </c>
-      <c r="G23" s="2" t="s">
-        <v>49</v>
       </c>
       <c r="H23" s="2" t="s">
         <v>19</v>
@@ -1373,10 +1373,10 @@
         <v>20</v>
       </c>
       <c r="J23" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="K23" s="2" t="s">
         <v>52</v>
-      </c>
-      <c r="K23" s="2" t="s">
-        <v>53</v>
       </c>
       <c r="L23" s="2" t="s">
         <v>22</v>
@@ -1395,10 +1395,10 @@
       <c r="H24" s="9"/>
       <c r="I24" s="9"/>
       <c r="J24" s="7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="K24" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="L24" s="7" t="s">
         <v>22</v>
@@ -1415,10 +1415,10 @@
       <c r="H25" s="9"/>
       <c r="I25" s="9"/>
       <c r="J25" s="7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="K25" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="L25" s="7" t="s">
         <v>22</v>
@@ -1435,10 +1435,10 @@
       <c r="H26" s="9"/>
       <c r="I26" s="9"/>
       <c r="J26" s="7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="K26" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="L26" s="7" t="s">
         <v>22</v>
@@ -1455,10 +1455,10 @@
       <c r="H27" s="9"/>
       <c r="I27" s="9"/>
       <c r="J27" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="K27" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="L27" s="7" t="s">
         <v>22</v>
@@ -1475,10 +1475,10 @@
       <c r="H28" s="9"/>
       <c r="I28" s="9"/>
       <c r="J28" s="7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="K28" s="7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="L28" s="7" t="s">
         <v>22</v>
@@ -1495,10 +1495,10 @@
       <c r="H29" s="9"/>
       <c r="I29" s="9"/>
       <c r="J29" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="K29" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="L29" s="7" t="s">
         <v>22</v>
@@ -1515,10 +1515,10 @@
       <c r="H30" s="9"/>
       <c r="I30" s="9"/>
       <c r="J30" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="K30" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="L30" s="7" t="s">
         <v>22</v>
@@ -1535,10 +1535,10 @@
       <c r="H31" s="3"/>
       <c r="I31" s="3"/>
       <c r="J31" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="K31" s="4" t="s">
         <v>68</v>
-      </c>
-      <c r="K31" s="4" t="s">
-        <v>69</v>
       </c>
       <c r="L31" s="4" t="s">
         <v>22</v>

</xml_diff>